<commit_message>
Links de clases actualizados
</commit_message>
<xml_diff>
--- a/Material Práctico/ISW2020_LINK_CLASES_PRACTICAS.xlsx
+++ b/Material Práctico/ISW2020_LINK_CLASES_PRACTICAS.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mromero\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matias\Desktop\Repo\ISW_2020_4K3_GRUPO_08\Material Práctico\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D4431BFC-899F-4E46-8CE4-B53037D1B966}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{3E4279B0-F49B-4F45-9D80-45A5F7B23C22}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="19425" windowHeight="10425"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="41">
   <si>
     <t>Filosofia agil</t>
   </si>
@@ -99,12 +98,69 @@
   </si>
   <si>
     <t>LINK</t>
+  </si>
+  <si>
+    <t>Scrum</t>
+  </si>
+  <si>
+    <t>https://youtu.be/q0QL9jbSx4c</t>
+  </si>
+  <si>
+    <t>https://youtu.be/V85VSxP9Hz4</t>
+  </si>
+  <si>
+    <t>https://youtu.be/KXtjGzz-AwM</t>
+  </si>
+  <si>
+    <t>Sprint</t>
+  </si>
+  <si>
+    <t>https://youtu.be/sjpEWQ61R5o</t>
+  </si>
+  <si>
+    <t>https://youtu.be/C5FVpLiZA24</t>
+  </si>
+  <si>
+    <t>Testing de Caja Negra</t>
+  </si>
+  <si>
+    <t>https://youtu.be/OUY0N9cuz18</t>
+  </si>
+  <si>
+    <t>https://youtu.be/QJkThF0MpDs</t>
+  </si>
+  <si>
+    <t>Testing Caja Blanca</t>
+  </si>
+  <si>
+    <t>https://youtu.be/5kfUgtONLE0</t>
+  </si>
+  <si>
+    <t>https://youtu.be/o0IJSCVb7t8</t>
+  </si>
+  <si>
+    <t>Ejecución de Casos de Prueba</t>
+  </si>
+  <si>
+    <t>https://youtu.be/4sxrbciyBZY</t>
+  </si>
+  <si>
+    <t>Repaso para el parcial</t>
+  </si>
+  <si>
+    <t>https://youtu.be/jK4MykdHH40</t>
+  </si>
+  <si>
+    <t>Practico 13 Design Thinking</t>
+  </si>
+  <si>
+    <t>https://youtu.be/ZLYnX0E4Uf4</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -149,7 +205,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -163,9 +219,17 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -477,21 +541,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C6097CFC-8F10-44D3-8FC1-A9AF0B4A7B63}">
-  <dimension ref="A2:E18"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:E36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="F41" sqref="F41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.36328125" customWidth="1"/>
-    <col min="2" max="2" width="29.6328125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="74.6328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.42578125" customWidth="1"/>
+    <col min="2" max="2" width="29.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="74.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>18</v>
       </c>
@@ -505,7 +569,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>43959</v>
       </c>
@@ -520,7 +584,7 @@
       </c>
       <c r="E3" s="2"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="3"/>
       <c r="B4" s="2"/>
       <c r="C4" s="3">
@@ -531,7 +595,7 @@
       </c>
       <c r="E4" s="2"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="3"/>
       <c r="B5" s="2"/>
       <c r="C5" s="3">
@@ -542,14 +606,14 @@
       </c>
       <c r="E5" s="2"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="3"/>
       <c r="B6" s="2"/>
       <c r="C6" s="3"/>
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>44173</v>
       </c>
@@ -564,7 +628,7 @@
       </c>
       <c r="E7" s="2"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="3"/>
       <c r="B8" s="2"/>
       <c r="C8" s="3">
@@ -575,7 +639,7 @@
       </c>
       <c r="E8" s="2"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="3"/>
       <c r="B9" s="2"/>
       <c r="C9" s="3">
@@ -586,7 +650,7 @@
       </c>
       <c r="E9" s="2"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="3"/>
       <c r="B10" s="2"/>
       <c r="C10" s="3">
@@ -597,14 +661,14 @@
       </c>
       <c r="E10" s="2"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="3"/>
       <c r="B11" s="2"/>
       <c r="C11" s="3"/>
       <c r="D11" s="2"/>
       <c r="E11" s="2"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>9</v>
       </c>
@@ -619,7 +683,7 @@
       </c>
       <c r="E12" s="2"/>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="3"/>
       <c r="B13" s="2"/>
       <c r="C13" s="3">
@@ -630,7 +694,7 @@
       </c>
       <c r="E13" s="2"/>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="3"/>
       <c r="B14" s="2"/>
       <c r="C14" s="3">
@@ -641,14 +705,14 @@
       </c>
       <c r="E14" s="2"/>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="3"/>
       <c r="B15" s="2"/>
       <c r="C15" s="3"/>
       <c r="D15" s="2"/>
       <c r="E15" s="2"/>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>14</v>
       </c>
@@ -663,7 +727,7 @@
       </c>
       <c r="E16" s="2"/>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="3"/>
       <c r="B17" s="2"/>
       <c r="C17" s="3">
@@ -674,27 +738,177 @@
       </c>
       <c r="E17" s="2"/>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="3"/>
       <c r="B18" s="2"/>
       <c r="C18" s="3"/>
       <c r="D18" s="2"/>
       <c r="E18" s="2"/>
     </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="5">
+        <v>44076</v>
+      </c>
+      <c r="B19" t="s">
+        <v>22</v>
+      </c>
+      <c r="C19" s="3">
+        <v>1</v>
+      </c>
+      <c r="D19" s="6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C20" s="3">
+        <v>2</v>
+      </c>
+      <c r="D20" s="6" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C21" s="3">
+        <v>3</v>
+      </c>
+      <c r="D21" s="6" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="7">
+        <v>44083</v>
+      </c>
+      <c r="B23" t="s">
+        <v>26</v>
+      </c>
+      <c r="C23" s="3">
+        <v>1</v>
+      </c>
+      <c r="D23" s="6" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C24" s="3">
+        <v>2</v>
+      </c>
+      <c r="D24" s="6" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" s="7">
+        <v>44090</v>
+      </c>
+      <c r="B26" t="s">
+        <v>29</v>
+      </c>
+      <c r="C26" s="3">
+        <v>1</v>
+      </c>
+      <c r="D26" s="6" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C27" s="3">
+        <v>2</v>
+      </c>
+      <c r="D27" s="6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" s="7">
+        <v>44097</v>
+      </c>
+      <c r="B29" t="s">
+        <v>32</v>
+      </c>
+      <c r="C29" s="3">
+        <v>1</v>
+      </c>
+      <c r="D29" s="6" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C30" s="3">
+        <v>2</v>
+      </c>
+      <c r="D30" s="6" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" s="7">
+        <v>44111</v>
+      </c>
+      <c r="B32" t="s">
+        <v>35</v>
+      </c>
+      <c r="C32" s="3">
+        <v>1</v>
+      </c>
+      <c r="D32" s="6" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" s="7">
+        <v>37544</v>
+      </c>
+      <c r="B34" t="s">
+        <v>37</v>
+      </c>
+      <c r="C34" s="3">
+        <v>1</v>
+      </c>
+      <c r="D34" s="6" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" s="7">
+        <v>44125</v>
+      </c>
+      <c r="B36" t="s">
+        <v>39</v>
+      </c>
+      <c r="C36" s="8">
+        <v>1</v>
+      </c>
+      <c r="D36" s="6" t="s">
+        <v>40</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D4" r:id="rId1" xr:uid="{C6438B1C-73F4-498A-B061-3ABA62795411}"/>
-    <hyperlink ref="D7" r:id="rId2" xr:uid="{12097BD9-7217-4847-A80D-98B76206AFB4}"/>
-    <hyperlink ref="D13" r:id="rId3" xr:uid="{86467CBD-1212-4D82-885B-96464A54B9D4}"/>
-    <hyperlink ref="D16" r:id="rId4" xr:uid="{84E745C6-5425-4372-B136-B2023AD29EE5}"/>
-    <hyperlink ref="D17" r:id="rId5" xr:uid="{884B1800-9BA2-4648-8CE9-1E0CAE6C9DF8}"/>
-    <hyperlink ref="D14" r:id="rId6" xr:uid="{9564DA24-3E0A-4C87-8EBA-04E3CC178AA9}"/>
-    <hyperlink ref="D12" r:id="rId7" xr:uid="{CEBA217C-A64F-4900-8E54-552D9F4AAE4C}"/>
-    <hyperlink ref="D3" r:id="rId8" xr:uid="{0B67AEC8-395D-4279-AF43-65E73B32B8D1}"/>
-    <hyperlink ref="D5" r:id="rId9" xr:uid="{208BC4CD-C5E5-4D41-A86B-BC8D461FD11D}"/>
-    <hyperlink ref="D8" r:id="rId10" xr:uid="{53ACC2C2-E79C-4C83-9CA0-E7024511A456}"/>
-    <hyperlink ref="D10" r:id="rId11" xr:uid="{A22A9742-4DC5-4EEC-B4D9-041525EC5960}"/>
-    <hyperlink ref="D9" r:id="rId12" xr:uid="{3A86A439-DB9F-464C-B7AA-F1E522F2ECE9}"/>
+    <hyperlink ref="D4" r:id="rId1"/>
+    <hyperlink ref="D7" r:id="rId2"/>
+    <hyperlink ref="D13" r:id="rId3"/>
+    <hyperlink ref="D16" r:id="rId4"/>
+    <hyperlink ref="D17" r:id="rId5"/>
+    <hyperlink ref="D14" r:id="rId6"/>
+    <hyperlink ref="D12" r:id="rId7"/>
+    <hyperlink ref="D3" r:id="rId8"/>
+    <hyperlink ref="D5" r:id="rId9"/>
+    <hyperlink ref="D8" r:id="rId10"/>
+    <hyperlink ref="D10" r:id="rId11"/>
+    <hyperlink ref="D9" r:id="rId12"/>
+    <hyperlink ref="D19" r:id="rId13"/>
+    <hyperlink ref="D20" r:id="rId14"/>
+    <hyperlink ref="D21" r:id="rId15"/>
+    <hyperlink ref="D23" r:id="rId16"/>
+    <hyperlink ref="D24" r:id="rId17"/>
+    <hyperlink ref="D26" r:id="rId18"/>
+    <hyperlink ref="D27" r:id="rId19"/>
+    <hyperlink ref="D29" r:id="rId20"/>
+    <hyperlink ref="D30" r:id="rId21"/>
+    <hyperlink ref="D32" r:id="rId22"/>
+    <hyperlink ref="D34" r:id="rId23"/>
+    <hyperlink ref="D36" r:id="rId24"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>